<commit_message>
added test for file with 2 sheets
</commit_message>
<xml_diff>
--- a/ExcelExamples/ExcelFileExtract/test.xlsx
+++ b/ExcelExamples/ExcelFileExtract/test.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\OneDrive\jorgeprg\csharp\examples\ExcelExamples\ExcelExamples\ExcelExamples\ExcelFileExtract\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e1073935\Downloads\ExcelSample\ExcelExamples\ExcelFileExtract\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5C3C8207-7FA7-475B-987F-6FD044B9E21F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" xr2:uid="{576C7B85-F639-430A-9B1E-0EAC7A385261}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6828" activeTab="1" xr2:uid="{576C7B85-F639-430A-9B1E-0EAC7A385261}"/>
   </bookViews>
   <sheets>
     <sheet name="testing" sheetId="1" r:id="rId1"/>
+    <sheet name="testing2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="6">
   <si>
     <t>sssd</t>
   </si>
@@ -49,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,8 +57,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -68,6 +75,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -84,10 +97,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,26 +416,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430F219D-FFAC-4A40-B250-04DC89E98530}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -429,7 +446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -437,7 +454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -445,7 +462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -457,4 +474,65 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C41075-9FC1-452E-8758-51BF0041CBA0}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>